<commit_message>
Sửa export dssv + layout
</commit_message>
<xml_diff>
--- a/04.Source/CapstoneMVC/src/main/resources/template/DSSV.xlsx
+++ b/04.Source/CapstoneMVC/src/main/resources/template/DSSV.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Projects\Intelliji\CapstoneRoot\04.Source\CapstoneMVC\src\main\resources\template\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="6705"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Danh sách các môn trong Curriculum</t>
   </si>
@@ -45,12 +40,15 @@
   </si>
   <si>
     <t>Khung chương trình</t>
+  </si>
+  <si>
+    <t>Ngành học</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -197,7 +195,7 @@
         <xdr:cNvPr id="6" name="Picture 5" descr="New Logo - Update01">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -511,7 +509,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -519,24 +517,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="24" style="3" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="3" customWidth="1"/>
     <col min="5" max="5" width="26.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="22.42578125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="5" t="s">
@@ -544,31 +543,31 @@
       </c>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -576,15 +575,18 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Export sv giỏi + sửa bug
</commit_message>
<xml_diff>
--- a/04.Source/CapstoneMVC/src/main/resources/template/DSSV.xlsx
+++ b/04.Source/CapstoneMVC/src/main/resources/template/DSSV.xlsx
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>Danh sách các môn trong Curriculum</t>
-  </si>
-  <si>
     <t>Học kỳ</t>
   </si>
   <si>
@@ -43,6 +40,9 @@
   </si>
   <si>
     <t>Ngành học</t>
+  </si>
+  <si>
+    <t>Danh sách sinh viên</t>
   </si>
 </sst>
 </file>
@@ -195,7 +195,7 @@
         <xdr:cNvPr id="6" name="Picture 5" descr="New Logo - Update01">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -509,7 +509,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -520,7 +520,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +539,7 @@
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="5" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D1" s="5"/>
     </row>
@@ -569,25 +569,25 @@
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>